<commit_message>
Thanh Tran - Update Technical Require
</commit_message>
<xml_diff>
--- a/Requirement/Requirement Document.xlsx
+++ b/Requirement/Requirement Document.xlsx
@@ -115,9 +115,6 @@
     <t xml:space="preserve">Framework </t>
   </si>
   <si>
-    <t>Spring MVC, Spring Boot</t>
-  </si>
-  <si>
     <t>Node js</t>
   </si>
   <si>
@@ -125,6 +122,9 @@
   </si>
   <si>
     <t>PostgresSQL</t>
+  </si>
+  <si>
+    <t>Spring MVC</t>
   </si>
 </sst>
 </file>
@@ -469,7 +469,7 @@
   <dimension ref="B2:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +614,7 @@
         <v>32</v>
       </c>
       <c r="D27" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.25">
@@ -646,15 +646,15 @@
         <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" t="s">
         <v>35</v>
-      </c>
-      <c r="D32" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>